<commit_message>
added power measurements NFC node
</commit_message>
<xml_diff>
--- a/hardware/OctaSensor/OctaSensor/BOM_Octa_Sensor.xlsx
+++ b/hardware/OctaSensor/OctaSensor/BOM_Octa_Sensor.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32910" windowHeight="14265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Basic_OCTA-MINI" sheetId="1" r:id="rId1"/>
@@ -1101,15 +1101,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.140625" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>

</xml_diff>